<commit_message>
Code refactoring of project files
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nodeproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jsdev\nodeproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -249,7 +249,7 @@
     <t>24.06.2022</t>
   </si>
   <si>
-    <t>11.07.2022</t>
+    <t>16.07.2022</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1073,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>